<commit_message>
Actualizar paso1.py y listado jira iso.xlsx
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/isoReport/docs/listado jira iso.xlsx
+++ b/isoReport/docs/listado jira iso.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aagricola-my.sharepoint.com/personal/inavarro_atlanticaagricola_com/Documents/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aagricola-my.sharepoint.com/personal/inavarro_atlanticaagricola_com/Documents/Escritorio/Repos/isoReport/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{3196883F-C5CC-444C-8837-DDEB28769FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0855E048-4881-4B17-8CD2-8C29C9B8D001}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{3196883F-C5CC-444C-8837-DDEB28769FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BC5E636-0C98-4157-A675-21D94A97A308}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" activeTab="2" xr2:uid="{190B92D9-6C2C-4795-950E-F3420A92F605}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{190B92D9-6C2C-4795-950E-F3420A92F605}"/>
   </bookViews>
   <sheets>
     <sheet name="Jira" sheetId="2" r:id="rId1"/>
@@ -3206,14 +3206,14 @@
   <autoFilter ref="A1:I145" xr:uid="{CEE3B5D2-3242-4D54-8CBB-04F1C23D0F60}"/>
   <tableColumns count="9">
     <tableColumn id="20" xr3:uid="{0E1A6E59-696C-4565-85FC-DBF5D0F778B1}" uniqueName="20" name="Orden" queryTableFieldId="20" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{952706E9-E32F-4695-8553-430A2487CC64}" uniqueName="5" name="ProyectoID" queryTableFieldId="5" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{265A3DF8-9EEC-460E-9C82-B86FB3CC2365}" uniqueName="2" name="Clave de incidencia" queryTableFieldId="2" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{35E05AA2-F76F-4CBB-A17D-9BF835608F8F}" uniqueName="4" name="Resumen" queryTableFieldId="4" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{6D294C6D-24E6-463D-920A-A410716BC064}" uniqueName="8" name="Estado" queryTableFieldId="8" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{DCC5E29B-9D5D-4A56-ADD6-9BE1F7B49FB1}" uniqueName="9" name="Creada" queryTableFieldId="9" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{8046135A-73D1-4323-8128-F88C5C6895D8}" uniqueName="10" name="Fecha de vencimiento" queryTableFieldId="10" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{F24BE980-76AA-4F7C-8C40-933213D341C5}" uniqueName="11" name="Actualizada" queryTableFieldId="11" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{01C51DA8-FB2F-4F6A-8434-7FFAB9B21336}" uniqueName="12" name="Resuelta" queryTableFieldId="12" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{952706E9-E32F-4695-8553-430A2487CC64}" uniqueName="5" name="ProyectoID" queryTableFieldId="5" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{265A3DF8-9EEC-460E-9C82-B86FB3CC2365}" uniqueName="2" name="Clave de incidencia" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{35E05AA2-F76F-4CBB-A17D-9BF835608F8F}" uniqueName="4" name="Resumen" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{6D294C6D-24E6-463D-920A-A410716BC064}" uniqueName="8" name="Estado" queryTableFieldId="8" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{DCC5E29B-9D5D-4A56-ADD6-9BE1F7B49FB1}" uniqueName="9" name="Creada" queryTableFieldId="9" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{8046135A-73D1-4323-8128-F88C5C6895D8}" uniqueName="10" name="Fecha de vencimiento" queryTableFieldId="10" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{F24BE980-76AA-4F7C-8C40-933213D341C5}" uniqueName="11" name="Actualizada" queryTableFieldId="11" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{01C51DA8-FB2F-4F6A-8434-7FFAB9B21336}" uniqueName="12" name="Resuelta" queryTableFieldId="12" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20282,8 +20282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5FBFF1-572B-4947-868E-B30B37170675}">
   <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Actualizar app.py, editor_ui.py, paso1.py y listado jira iso
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/isoReport/docs/listado jira iso.xlsx
+++ b/isoReport/docs/listado jira iso.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aagricola-my.sharepoint.com/personal/inavarro_atlanticaagricola_com/Documents/Escritorio/Repos/isoReport/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{3196883F-C5CC-444C-8837-DDEB28769FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BC5E636-0C98-4157-A675-21D94A97A308}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{3196883F-C5CC-444C-8837-DDEB28769FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07A9941F-38A8-4107-97C5-F339E0EF510B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{190B92D9-6C2C-4795-950E-F3420A92F605}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{190B92D9-6C2C-4795-950E-F3420A92F605}"/>
   </bookViews>
   <sheets>
     <sheet name="Jira" sheetId="2" r:id="rId1"/>
-    <sheet name="paso1" sheetId="1" r:id="rId2"/>
-    <sheet name="paso2" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId2"/>
+    <sheet name="paso1" sheetId="1" r:id="rId3"/>
+    <sheet name="paso2" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Jira!$A$1:$S$145</definedName>
-    <definedName name="DatosExternos_1" localSheetId="1" hidden="1">paso1!$B$1:$R$145</definedName>
-    <definedName name="DatosExternos_1" localSheetId="2" hidden="1">paso2!$B$1:$I$145</definedName>
+    <definedName name="DatosExternos_1" localSheetId="2" hidden="1">paso1!$B$1:$R$145</definedName>
+    <definedName name="DatosExternos_1" localSheetId="3" hidden="1">paso2!$B$1:$I$145</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6238" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6288" uniqueCount="868">
   <si>
     <t>Tipo de Incidencia</t>
   </si>
@@ -2860,7 +2861,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2868,16 +2869,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2885,12 +2906,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3538,8 +3573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDB59F-6B92-4BCE-8CA7-E7EF224B53D3}">
   <dimension ref="A1:S145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12125,6 +12160,271 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77145A30-7E7D-4358-BDDB-B62323BD4B7A}">
+  <dimension ref="A1:A50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AD4B66-8853-40EC-9636-B6B13888AA77}">
   <dimension ref="A1:R145"/>
   <sheetViews>
@@ -20278,11 +20578,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5FBFF1-572B-4947-868E-B30B37170675}">
   <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualizar paso1.py, BBDD CSV, listado jira y solicitudes 2025
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/isoReport/docs/listado jira iso.xlsx
+++ b/isoReport/docs/listado jira iso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aagricola-my.sharepoint.com/personal/inavarro_atlanticaagricola_com/Documents/Escritorio/Repos/isoReport/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{3196883F-C5CC-444C-8837-DDEB28769FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07A9941F-38A8-4107-97C5-F339E0EF510B}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{3196883F-C5CC-444C-8837-DDEB28769FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8CE3C13-C146-4DA1-BFFF-467E3F9B72E1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{190B92D9-6C2C-4795-950E-F3420A92F605}"/>
+    <workbookView minimized="1" xWindow="3480" yWindow="6840" windowWidth="7080" windowHeight="4080" xr2:uid="{190B92D9-6C2C-4795-950E-F3420A92F605}"/>
   </bookViews>
   <sheets>
     <sheet name="Jira" sheetId="2" r:id="rId1"/>
@@ -2923,8 +2923,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3177,7 +3177,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DAC8D5F-F972-4D80-8E57-29DD8308FB06}" name="Jira" displayName="Jira" ref="A1:S145" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:S145" xr:uid="{6DAC8D5F-F972-4D80-8E57-29DD8308FB06}"/>
+  <autoFilter ref="A1:S145" xr:uid="{6DAC8D5F-F972-4D80-8E57-29DD8308FB06}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="FOLICAT ZNMO - MN"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S145">
     <sortCondition ref="B1:B145"/>
   </sortState>
@@ -3573,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDB59F-6B92-4BCE-8CA7-E7EF224B53D3}">
   <dimension ref="A1:S145"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3714,7 +3720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3773,7 +3779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3832,7 +3838,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3950,7 +3956,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -4009,7 +4015,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -4068,7 +4074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4245,7 +4251,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -4304,7 +4310,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -4363,7 +4369,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -4422,7 +4428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -4481,7 +4487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -4658,7 +4664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -4835,7 +4841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -4894,7 +4900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -4953,7 +4959,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -5012,7 +5018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -5071,7 +5077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -5130,7 +5136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -5189,7 +5195,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -5248,7 +5254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -5307,7 +5313,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -5366,7 +5372,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -5425,7 +5431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -5484,7 +5490,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -5543,7 +5549,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -5602,7 +5608,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -5661,7 +5667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -5720,7 +5726,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -5779,7 +5785,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -5838,7 +5844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -5897,7 +5903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -5956,7 +5962,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -6015,7 +6021,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -6074,7 +6080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -6133,7 +6139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -6192,7 +6198,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -6251,7 +6257,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -6310,7 +6316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -6369,7 +6375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -6428,7 +6434,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -6487,7 +6493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -6546,7 +6552,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -6605,7 +6611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -6664,7 +6670,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -6723,7 +6729,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -6782,7 +6788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -6841,7 +6847,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -6900,7 +6906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -6959,7 +6965,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -7018,7 +7024,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -7077,7 +7083,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -7136,7 +7142,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -7254,7 +7260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -7313,7 +7319,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -7372,7 +7378,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -7431,7 +7437,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -7490,7 +7496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -7549,7 +7555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -7608,7 +7614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -7667,7 +7673,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -7726,7 +7732,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -7785,7 +7791,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -7844,7 +7850,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -7903,7 +7909,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -7962,7 +7968,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>17</v>
       </c>
@@ -8021,7 +8027,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -8080,7 +8086,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -8139,7 +8145,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -8198,7 +8204,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -8257,7 +8263,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -8316,7 +8322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -8375,7 +8381,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -8434,7 +8440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -8493,7 +8499,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -8552,7 +8558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -8611,7 +8617,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -8670,7 +8676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -8729,7 +8735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -8788,7 +8794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -8847,7 +8853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>17</v>
       </c>
@@ -8906,7 +8912,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -8965,7 +8971,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -9024,7 +9030,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -9083,7 +9089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -9142,7 +9148,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -9201,7 +9207,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>17</v>
       </c>
@@ -9260,7 +9266,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>17</v>
       </c>
@@ -9319,7 +9325,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>17</v>
       </c>
@@ -9378,7 +9384,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -9437,7 +9443,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>17</v>
       </c>
@@ -9496,7 +9502,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>17</v>
       </c>
@@ -9555,7 +9561,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>17</v>
       </c>
@@ -9614,7 +9620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>17</v>
       </c>
@@ -9673,7 +9679,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -9732,7 +9738,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>17</v>
       </c>
@@ -9791,7 +9797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>17</v>
       </c>
@@ -9850,7 +9856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>17</v>
       </c>
@@ -9909,7 +9915,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>17</v>
       </c>
@@ -9968,7 +9974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>17</v>
       </c>
@@ -10027,7 +10033,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>17</v>
       </c>
@@ -10086,7 +10092,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>17</v>
       </c>
@@ -10145,7 +10151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>17</v>
       </c>
@@ -10204,7 +10210,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>17</v>
       </c>
@@ -10263,7 +10269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -10322,7 +10328,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>17</v>
       </c>
@@ -10381,7 +10387,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>17</v>
       </c>
@@ -10440,7 +10446,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>17</v>
       </c>
@@ -10499,7 +10505,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>17</v>
       </c>
@@ -10558,7 +10564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>17</v>
       </c>
@@ -10617,7 +10623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>17</v>
       </c>
@@ -10676,7 +10682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>17</v>
       </c>
@@ -10735,7 +10741,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>17</v>
       </c>
@@ -10794,7 +10800,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>17</v>
       </c>
@@ -10853,7 +10859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>17</v>
       </c>
@@ -10912,7 +10918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>17</v>
       </c>
@@ -10971,7 +10977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -11030,7 +11036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -11089,7 +11095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -11148,7 +11154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -11207,7 +11213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>17</v>
       </c>
@@ -11266,7 +11272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>17</v>
       </c>
@@ -11325,7 +11331,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>17</v>
       </c>
@@ -11384,7 +11390,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>17</v>
       </c>
@@ -11443,7 +11449,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>17</v>
       </c>
@@ -11502,7 +11508,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>17</v>
       </c>
@@ -11561,7 +11567,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>17</v>
       </c>
@@ -11620,7 +11626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>17</v>
       </c>
@@ -11679,7 +11685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>17</v>
       </c>
@@ -11738,7 +11744,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>17</v>
       </c>
@@ -11797,7 +11803,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>17</v>
       </c>
@@ -11856,7 +11862,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>17</v>
       </c>
@@ -11915,7 +11921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>17</v>
       </c>
@@ -11974,7 +11980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>17</v>
       </c>
@@ -12033,7 +12039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>17</v>
       </c>
@@ -12092,7 +12098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>17</v>
       </c>
@@ -12163,7 +12169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77145A30-7E7D-4358-BDDB-B62323BD4B7A}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A50"/>
     </sheetView>
   </sheetViews>

</xml_diff>